<commit_message>
Código operativo. Documentacion de métodos. Actualizacion de fichero de entorno conda (.yml)
</commit_message>
<xml_diff>
--- a/qfacies_v1/Data/Datagroups_example.xlsx
+++ b/qfacies_v1/Data/Datagroups_example.xlsx
@@ -635,16 +635,16 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D5" t="n">
-        <v>4.14</v>
+        <v>8.17</v>
       </c>
       <c r="E5" t="n">
-        <v>64.79000000000001</v>
+        <v>67.58</v>
       </c>
       <c r="F5" t="n">
-        <v>10.34</v>
+        <v>15.96</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -652,10 +652,10 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>19.22</v>
+        <v>35.92</v>
       </c>
       <c r="I5" t="n">
-        <v>97.06999999999999</v>
+        <v>58.65</v>
       </c>
     </row>
     <row r="6">
@@ -666,16 +666,16 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D6" t="n">
-        <v>2.06</v>
+        <v>8.9</v>
       </c>
       <c r="E6" t="n">
-        <v>12.06</v>
+        <v>63.34</v>
       </c>
       <c r="F6" t="n">
-        <v>8.369999999999999</v>
+        <v>20.34</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -683,10 +683,10 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>173.82</v>
+        <v>4.15</v>
       </c>
       <c r="I6" t="n">
-        <v>66.11</v>
+        <v>67.90000000000001</v>
       </c>
     </row>
     <row r="7">
@@ -697,23 +697,23 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="D7" t="n">
-        <v>1.16</v>
+        <v>6.25</v>
       </c>
       <c r="E7" t="n">
-        <v>0</v>
+        <v>38.05</v>
       </c>
       <c r="F7" t="n">
-        <v>6.95</v>
+        <v>17.74</v>
       </c>
       <c r="G7" t="inlineStr"/>
       <c r="H7" t="n">
-        <v>169.93</v>
+        <v>46.47</v>
       </c>
       <c r="I7" t="n">
-        <v>44.36</v>
+        <v>42.31</v>
       </c>
     </row>
     <row r="8">
@@ -728,16 +728,16 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D8" t="n">
-        <v>6.35</v>
+        <v>10.98</v>
       </c>
       <c r="E8" t="n">
-        <v>48.76</v>
+        <v>55.12</v>
       </c>
       <c r="F8" t="n">
-        <v>15.3</v>
+        <v>18.06</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -745,10 +745,10 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>165.42</v>
+        <v>156.13</v>
       </c>
       <c r="I8" t="n">
-        <v>85.76000000000001</v>
+        <v>76.45999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -1286,16 +1286,16 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D26" t="n">
-        <v>3.31</v>
+        <v>7.04</v>
       </c>
       <c r="E26" t="n">
-        <v>0</v>
+        <v>12.67</v>
       </c>
       <c r="F26" t="n">
-        <v>10.74</v>
+        <v>14.34</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1303,10 +1303,10 @@
         </is>
       </c>
       <c r="H26" t="n">
-        <v>26.38</v>
+        <v>18.43</v>
       </c>
       <c r="I26" t="n">
-        <v>71.03</v>
+        <v>70.06999999999999</v>
       </c>
     </row>
     <row r="27">
@@ -1317,16 +1317,16 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D27" t="n">
-        <v>2.75</v>
+        <v>8.94</v>
       </c>
       <c r="E27" t="n">
-        <v>0</v>
+        <v>24.67</v>
       </c>
       <c r="F27" t="n">
-        <v>9.73</v>
+        <v>19.52</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1334,10 +1334,10 @@
         </is>
       </c>
       <c r="H27" t="n">
-        <v>11.16</v>
+        <v>6.1</v>
       </c>
       <c r="I27" t="n">
-        <v>73.29000000000001</v>
+        <v>44.18</v>
       </c>
     </row>
     <row r="28">
@@ -1348,23 +1348,23 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D28" t="n">
-        <v>2.69</v>
+        <v>5.33</v>
       </c>
       <c r="E28" t="n">
-        <v>0</v>
+        <v>12.67</v>
       </c>
       <c r="F28" t="n">
-        <v>12.89</v>
+        <v>16.17</v>
       </c>
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="n">
-        <v>48.07</v>
+        <v>34.11</v>
       </c>
       <c r="I28" t="n">
-        <v>26.99</v>
+        <v>31.24</v>
       </c>
     </row>
     <row r="29">
@@ -1379,16 +1379,16 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="D29" t="n">
-        <v>0.22</v>
+        <v>1.1</v>
       </c>
       <c r="E29" t="n">
-        <v>0</v>
+        <v>46.86</v>
       </c>
       <c r="F29" t="n">
-        <v>4.26</v>
+        <v>9.42</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1396,10 +1396,10 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>53.59</v>
+        <v>52.98</v>
       </c>
       <c r="I29" t="n">
-        <v>29.63</v>
+        <v>26.62</v>
       </c>
     </row>
     <row r="30">
@@ -1410,16 +1410,16 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="D30" t="n">
-        <v>1.11</v>
+        <v>2.06</v>
       </c>
       <c r="E30" t="n">
         <v>0</v>
       </c>
       <c r="F30" t="n">
-        <v>5.33</v>
+        <v>6.92</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1427,10 +1427,10 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>33.65</v>
+        <v>34.55</v>
       </c>
       <c r="I30" t="n">
-        <v>92.63</v>
+        <v>91.28</v>
       </c>
     </row>
     <row r="31">
@@ -1441,23 +1441,23 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D31" t="n">
-        <v>0.27</v>
+        <v>0.46</v>
       </c>
       <c r="E31" t="n">
         <v>0</v>
       </c>
       <c r="F31" t="n">
-        <v>4.38</v>
+        <v>5.4</v>
       </c>
       <c r="G31" t="inlineStr"/>
       <c r="H31" t="n">
-        <v>53.75</v>
+        <v>51.94</v>
       </c>
       <c r="I31" t="n">
-        <v>27.73</v>
+        <v>27.28</v>
       </c>
     </row>
   </sheetData>
@@ -1639,34 +1639,70 @@
           <t>841-7-0037</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="B4" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" t="n">
+        <v>7.18</v>
+      </c>
+      <c r="D4" t="n">
+        <v>64</v>
+      </c>
+      <c r="E4" t="n">
+        <v>24.69</v>
+      </c>
       <c r="F4" t="inlineStr">
         <is>
           <t>Chloride</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="inlineStr"/>
-      <c r="I4" t="inlineStr"/>
-      <c r="J4" t="inlineStr"/>
-      <c r="K4" t="inlineStr"/>
-      <c r="L4" t="inlineStr"/>
+      <c r="G4" t="n">
+        <v>10.4</v>
+      </c>
+      <c r="H4" t="n">
+        <v>75.44</v>
+      </c>
+      <c r="I4" t="n">
+        <v>5</v>
+      </c>
+      <c r="J4" t="n">
+        <v>9.119999999999999</v>
+      </c>
+      <c r="K4" t="n">
+        <v>85.33</v>
+      </c>
+      <c r="L4" t="n">
+        <v>29.68</v>
+      </c>
       <c r="M4" t="inlineStr">
         <is>
           <t>Sodium-Potassium-Mixed</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr"/>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr"/>
-      <c r="Q4" t="inlineStr"/>
-      <c r="R4" t="inlineStr"/>
-      <c r="S4" t="inlineStr"/>
-      <c r="T4" t="inlineStr"/>
-      <c r="U4" t="inlineStr"/>
+      <c r="N4" t="n">
+        <v>9.41</v>
+      </c>
+      <c r="O4" t="n">
+        <v>60.68</v>
+      </c>
+      <c r="P4" t="n">
+        <v>5</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>1.95</v>
+      </c>
+      <c r="R4" t="n">
+        <v>64</v>
+      </c>
+      <c r="S4" t="n">
+        <v>20.8</v>
+      </c>
+      <c r="T4" t="n">
+        <v>178.47</v>
+      </c>
+      <c r="U4" t="n">
+        <v>20.51</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1674,34 +1710,70 @@
           <t>841-4-0001</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>29</v>
+      </c>
+      <c r="C5" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="D5" t="n">
+        <v>63.34</v>
+      </c>
+      <c r="E5" t="n">
+        <v>20.34</v>
+      </c>
       <c r="F5" t="inlineStr">
         <is>
           <t>Chloride</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr"/>
-      <c r="H5" t="inlineStr"/>
-      <c r="I5" t="inlineStr"/>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
-      <c r="L5" t="inlineStr"/>
+      <c r="G5" t="n">
+        <v>4.15</v>
+      </c>
+      <c r="H5" t="n">
+        <v>67.90000000000001</v>
+      </c>
+      <c r="I5" t="n">
+        <v>29</v>
+      </c>
+      <c r="J5" t="n">
+        <v>8.17</v>
+      </c>
+      <c r="K5" t="n">
+        <v>67.58</v>
+      </c>
+      <c r="L5" t="n">
+        <v>15.96</v>
+      </c>
       <c r="M5" t="inlineStr">
         <is>
           <t>Mixed</t>
         </is>
       </c>
-      <c r="N5" t="inlineStr"/>
-      <c r="O5" t="inlineStr"/>
-      <c r="P5" t="inlineStr"/>
-      <c r="Q5" t="inlineStr"/>
-      <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
-      <c r="T5" t="inlineStr"/>
-      <c r="U5" t="inlineStr"/>
+      <c r="N5" t="n">
+        <v>35.92</v>
+      </c>
+      <c r="O5" t="n">
+        <v>58.65</v>
+      </c>
+      <c r="P5" t="n">
+        <v>29</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>6.25</v>
+      </c>
+      <c r="R5" t="n">
+        <v>38.05</v>
+      </c>
+      <c r="S5" t="n">
+        <v>17.74</v>
+      </c>
+      <c r="T5" t="n">
+        <v>46.47</v>
+      </c>
+      <c r="U5" t="n">
+        <v>42.31</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1709,34 +1781,70 @@
           <t>841-7-0006</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>22</v>
+      </c>
+      <c r="C6" t="n">
+        <v>19.54</v>
+      </c>
+      <c r="D6" t="n">
+        <v>79.76000000000001</v>
+      </c>
+      <c r="E6" t="n">
+        <v>30.26</v>
+      </c>
       <c r="F6" t="inlineStr">
         <is>
           <t>Chloride</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="inlineStr"/>
-      <c r="J6" t="inlineStr"/>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
+      <c r="G6" t="n">
+        <v>5.26</v>
+      </c>
+      <c r="H6" t="n">
+        <v>84.03</v>
+      </c>
+      <c r="I6" t="n">
+        <v>22</v>
+      </c>
+      <c r="J6" t="n">
+        <v>10.98</v>
+      </c>
+      <c r="K6" t="n">
+        <v>55.12</v>
+      </c>
+      <c r="L6" t="n">
+        <v>18.06</v>
+      </c>
       <c r="M6" t="inlineStr">
         <is>
           <t>Mixed</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr"/>
-      <c r="O6" t="inlineStr"/>
-      <c r="P6" t="inlineStr"/>
-      <c r="Q6" t="inlineStr"/>
-      <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
-      <c r="T6" t="inlineStr"/>
-      <c r="U6" t="inlineStr"/>
+      <c r="N6" t="n">
+        <v>156.13</v>
+      </c>
+      <c r="O6" t="n">
+        <v>76.45999999999999</v>
+      </c>
+      <c r="P6" t="n">
+        <v>22</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>11</v>
+      </c>
+      <c r="R6" t="n">
+        <v>86.5</v>
+      </c>
+      <c r="S6" t="n">
+        <v>23.45</v>
+      </c>
+      <c r="T6" t="n">
+        <v>26.56</v>
+      </c>
+      <c r="U6" t="n">
+        <v>45.16</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1744,34 +1852,70 @@
           <t>841-8-0017</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr"/>
-      <c r="C7" t="inlineStr"/>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="B7" t="n">
+        <v>14</v>
+      </c>
+      <c r="C7" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>72.14</v>
+      </c>
+      <c r="E7" t="n">
+        <v>22.88</v>
+      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>Chloride</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
-      <c r="I7" t="inlineStr"/>
-      <c r="J7" t="inlineStr"/>
-      <c r="K7" t="inlineStr"/>
-      <c r="L7" t="inlineStr"/>
+      <c r="G7" t="n">
+        <v>4.59</v>
+      </c>
+      <c r="H7" t="n">
+        <v>34.18</v>
+      </c>
+      <c r="I7" t="n">
+        <v>14</v>
+      </c>
+      <c r="J7" t="n">
+        <v>3.01</v>
+      </c>
+      <c r="K7" t="n">
+        <v>61.71</v>
+      </c>
+      <c r="L7" t="n">
+        <v>12.78</v>
+      </c>
       <c r="M7" t="inlineStr">
         <is>
           <t>Mixed</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
-      <c r="O7" t="inlineStr"/>
-      <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr"/>
-      <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
-      <c r="T7" t="inlineStr"/>
-      <c r="U7" t="inlineStr"/>
+      <c r="N7" t="n">
+        <v>12.28</v>
+      </c>
+      <c r="O7" t="n">
+        <v>84.45999999999999</v>
+      </c>
+      <c r="P7" t="n">
+        <v>14</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="R7" t="n">
+        <v>61.22</v>
+      </c>
+      <c r="S7" t="n">
+        <v>17.36</v>
+      </c>
+      <c r="T7" t="n">
+        <v>35.14</v>
+      </c>
+      <c r="U7" t="n">
+        <v>26.63</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
@@ -1779,34 +1923,70 @@
           <t>841-7-0038</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr"/>
-      <c r="C8" t="inlineStr"/>
-      <c r="D8" t="inlineStr"/>
-      <c r="E8" t="inlineStr"/>
+      <c r="B8" t="n">
+        <v>20</v>
+      </c>
+      <c r="C8" t="n">
+        <v>9.52</v>
+      </c>
+      <c r="D8" t="n">
+        <v>45.33</v>
+      </c>
+      <c r="E8" t="n">
+        <v>31.84</v>
+      </c>
       <c r="F8" t="inlineStr">
         <is>
           <t>Chloride</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr"/>
-      <c r="J8" t="inlineStr"/>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="G8" t="n">
+        <v>177.11</v>
+      </c>
+      <c r="H8" t="n">
+        <v>37.21</v>
+      </c>
+      <c r="I8" t="n">
+        <v>20</v>
+      </c>
+      <c r="J8" t="n">
+        <v>15.07</v>
+      </c>
+      <c r="K8" t="n">
+        <v>84.67</v>
+      </c>
+      <c r="L8" t="n">
+        <v>27.03</v>
+      </c>
       <c r="M8" t="inlineStr">
         <is>
           <t>Sodium-Potassium</t>
         </is>
       </c>
-      <c r="N8" t="inlineStr"/>
-      <c r="O8" t="inlineStr"/>
-      <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr"/>
-      <c r="R8" t="inlineStr"/>
-      <c r="S8" t="inlineStr"/>
-      <c r="T8" t="inlineStr"/>
-      <c r="U8" t="inlineStr"/>
+      <c r="N8" t="n">
+        <v>179.69</v>
+      </c>
+      <c r="O8" t="n">
+        <v>77.75</v>
+      </c>
+      <c r="P8" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>15.21</v>
+      </c>
+      <c r="R8" t="n">
+        <v>78</v>
+      </c>
+      <c r="S8" t="n">
+        <v>32.15</v>
+      </c>
+      <c r="T8" t="n">
+        <v>17.96</v>
+      </c>
+      <c r="U8" t="n">
+        <v>36.81</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
@@ -1814,34 +1994,70 @@
           <t>841-7-0057</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>15</v>
+      </c>
+      <c r="C9" t="n">
+        <v>3.04</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E9" t="n">
+        <v>11.04</v>
+      </c>
       <c r="F9" t="inlineStr">
         <is>
           <t>Chloride</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
-      <c r="I9" t="inlineStr"/>
-      <c r="J9" t="inlineStr"/>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+      <c r="G9" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="H9" t="n">
+        <v>73.59999999999999</v>
+      </c>
+      <c r="I9" t="n">
+        <v>15</v>
+      </c>
+      <c r="J9" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" t="n">
+        <v>8.92</v>
+      </c>
       <c r="M9" t="inlineStr">
         <is>
           <t>Sodium-Potassium</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr"/>
-      <c r="O9" t="inlineStr"/>
-      <c r="P9" t="inlineStr"/>
-      <c r="Q9" t="inlineStr"/>
-      <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
-      <c r="T9" t="inlineStr"/>
-      <c r="U9" t="inlineStr"/>
+      <c r="N9" t="n">
+        <v>14.21</v>
+      </c>
+      <c r="O9" t="n">
+        <v>84.55</v>
+      </c>
+      <c r="P9" t="n">
+        <v>15</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0</v>
+      </c>
+      <c r="S9" t="n">
+        <v>10.48</v>
+      </c>
+      <c r="T9" t="n">
+        <v>38.57</v>
+      </c>
+      <c r="U9" t="n">
+        <v>37.83</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1849,34 +2065,70 @@
           <t>841-7-0068</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
-      <c r="E10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>17</v>
+      </c>
+      <c r="C10" t="n">
+        <v>4.08</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" t="n">
+        <v>13.62</v>
+      </c>
       <c r="F10" t="inlineStr">
         <is>
           <t>Chloride</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr"/>
-      <c r="H10" t="inlineStr"/>
-      <c r="I10" t="inlineStr"/>
-      <c r="J10" t="inlineStr"/>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="G10" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="H10" t="n">
+        <v>62.52</v>
+      </c>
+      <c r="I10" t="n">
+        <v>17</v>
+      </c>
+      <c r="J10" t="n">
+        <v>4.09</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" t="n">
+        <v>11.27</v>
+      </c>
       <c r="M10" t="inlineStr">
         <is>
           <t>Sodium-Potassium</t>
         </is>
       </c>
-      <c r="N10" t="inlineStr"/>
-      <c r="O10" t="inlineStr"/>
-      <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr"/>
-      <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
-      <c r="T10" t="inlineStr"/>
-      <c r="U10" t="inlineStr"/>
+      <c r="N10" t="n">
+        <v>175.98</v>
+      </c>
+      <c r="O10" t="n">
+        <v>93.3</v>
+      </c>
+      <c r="P10" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>3.61</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0</v>
+      </c>
+      <c r="S10" t="n">
+        <v>14.44</v>
+      </c>
+      <c r="T10" t="n">
+        <v>25.48</v>
+      </c>
+      <c r="U10" t="n">
+        <v>32.96</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -1884,34 +2136,70 @@
           <t>841-7-0081</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
-      <c r="E11" t="inlineStr"/>
+      <c r="B11" t="n">
+        <v>17</v>
+      </c>
+      <c r="C11" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="n">
+        <v>9.26</v>
+      </c>
       <c r="F11" t="inlineStr">
         <is>
           <t>Chloride</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr"/>
-      <c r="H11" t="inlineStr"/>
-      <c r="I11" t="inlineStr"/>
-      <c r="J11" t="inlineStr"/>
-      <c r="K11" t="inlineStr"/>
-      <c r="L11" t="inlineStr"/>
+      <c r="G11" t="n">
+        <v>176.28</v>
+      </c>
+      <c r="H11" t="n">
+        <v>64.91</v>
+      </c>
+      <c r="I11" t="n">
+        <v>17</v>
+      </c>
+      <c r="J11" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="K11" t="n">
+        <v>66.51000000000001</v>
+      </c>
+      <c r="L11" t="n">
+        <v>20.45</v>
+      </c>
       <c r="M11" t="inlineStr">
         <is>
           <t>Sodium-Potassium</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr"/>
-      <c r="O11" t="inlineStr"/>
-      <c r="P11" t="inlineStr"/>
-      <c r="Q11" t="inlineStr"/>
-      <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
-      <c r="T11" t="inlineStr"/>
-      <c r="U11" t="inlineStr"/>
+      <c r="N11" t="n">
+        <v>151.43</v>
+      </c>
+      <c r="O11" t="n">
+        <v>87.94</v>
+      </c>
+      <c r="P11" t="n">
+        <v>17</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="R11" t="n">
+        <v>66.44</v>
+      </c>
+      <c r="S11" t="n">
+        <v>20.21</v>
+      </c>
+      <c r="T11" t="n">
+        <v>119.33</v>
+      </c>
+      <c r="U11" t="n">
+        <v>32.72</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
@@ -1919,34 +2207,70 @@
           <t>841-8-0060</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
-      <c r="E12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>20</v>
+      </c>
+      <c r="C12" t="n">
+        <v>8.94</v>
+      </c>
+      <c r="D12" t="n">
+        <v>24.67</v>
+      </c>
+      <c r="E12" t="n">
+        <v>19.52</v>
+      </c>
       <c r="F12" t="inlineStr">
         <is>
           <t>Chloride</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr"/>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="inlineStr"/>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="H12" t="n">
+        <v>44.18</v>
+      </c>
+      <c r="I12" t="n">
+        <v>20</v>
+      </c>
+      <c r="J12" t="n">
+        <v>7.04</v>
+      </c>
+      <c r="K12" t="n">
+        <v>12.67</v>
+      </c>
+      <c r="L12" t="n">
+        <v>14.34</v>
+      </c>
       <c r="M12" t="inlineStr">
         <is>
           <t>Sodium-Potassium</t>
         </is>
       </c>
-      <c r="N12" t="inlineStr"/>
-      <c r="O12" t="inlineStr"/>
-      <c r="P12" t="inlineStr"/>
-      <c r="Q12" t="inlineStr"/>
-      <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
-      <c r="T12" t="inlineStr"/>
-      <c r="U12" t="inlineStr"/>
+      <c r="N12" t="n">
+        <v>18.43</v>
+      </c>
+      <c r="O12" t="n">
+        <v>70.06999999999999</v>
+      </c>
+      <c r="P12" t="n">
+        <v>20</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>5.33</v>
+      </c>
+      <c r="R12" t="n">
+        <v>12.67</v>
+      </c>
+      <c r="S12" t="n">
+        <v>16.17</v>
+      </c>
+      <c r="T12" t="n">
+        <v>34.11</v>
+      </c>
+      <c r="U12" t="n">
+        <v>31.24</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
@@ -1954,34 +2278,70 @@
           <t>1037-7-0005</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
+      <c r="B13" t="n">
+        <v>42</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" t="n">
+        <v>6.92</v>
+      </c>
       <c r="F13" t="inlineStr">
         <is>
           <t>Bicarbonate</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr"/>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr"/>
-      <c r="J13" t="inlineStr"/>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>34.55</v>
+      </c>
+      <c r="H13" t="n">
+        <v>91.28</v>
+      </c>
+      <c r="I13" t="n">
+        <v>42</v>
+      </c>
+      <c r="J13" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>46.86</v>
+      </c>
+      <c r="L13" t="n">
+        <v>9.42</v>
+      </c>
       <c r="M13" t="inlineStr">
         <is>
           <t>Calcium</t>
         </is>
       </c>
-      <c r="N13" t="inlineStr"/>
-      <c r="O13" t="inlineStr"/>
-      <c r="P13" t="inlineStr"/>
-      <c r="Q13" t="inlineStr"/>
-      <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
-      <c r="T13" t="inlineStr"/>
-      <c r="U13" t="inlineStr"/>
+      <c r="N13" t="n">
+        <v>52.98</v>
+      </c>
+      <c r="O13" t="n">
+        <v>26.62</v>
+      </c>
+      <c r="P13" t="n">
+        <v>42</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0</v>
+      </c>
+      <c r="S13" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="T13" t="n">
+        <v>51.94</v>
+      </c>
+      <c r="U13" t="n">
+        <v>27.28</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>